<commit_message>
Actualización Plan de Proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/Linea Base/02. Planeación/ControlDeGastos-PlanProyecto.xlsx
+++ b/Proyectos/ControlDeGastos/Linea Base/02. Planeación/ControlDeGastos-PlanProyecto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="8445" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="151">
   <si>
     <t>Plan de Proyecto</t>
   </si>
@@ -487,24 +487,9 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Presentación de Proyecto</t>
-  </si>
-  <si>
-    <t>Instalador</t>
-  </si>
-  <si>
     <t>Manual de Usuario</t>
   </si>
   <si>
-    <t>Manual para ayudar al usuario a dar uso sobre el sistema</t>
-  </si>
-  <si>
-    <t>Ejecutable de programa que instala el producto solicitado por el cliente en diversas máquinas</t>
-  </si>
-  <si>
-    <t>Mostrar al cliente equipo de trabajo y metodología para realizar el proyecto del cliente</t>
-  </si>
-  <si>
     <t>https://trello.com/b/4r1sCMqp/controlgastos</t>
   </si>
   <si>
@@ -535,18 +520,6 @@
     <t>mayra.tejeda@gmail.com</t>
   </si>
   <si>
-    <t>GitHub</t>
-  </si>
-  <si>
-    <t>Source Tree</t>
-  </si>
-  <si>
-    <t>Toggl</t>
-  </si>
-  <si>
-    <t>Vianey Castillo, Ignacio Martínez, Mayra Tejeda</t>
-  </si>
-  <si>
     <t>Equipo de Trabajo</t>
   </si>
   <si>
@@ -662,6 +635,15 @@
   </si>
   <si>
     <t>Qualtop</t>
+  </si>
+  <si>
+    <t>Validar la correcta transacción de sistema al cliente con su correcto funcionamiento</t>
+  </si>
+  <si>
+    <t>Software Implementado</t>
+  </si>
+  <si>
+    <t>Quincenal</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1566,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1828,9 +1810,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2087,6 +2066,12 @@
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2349,7 +2334,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3867150" y="5295900"/>
+          <a:off x="3867150" y="4810125"/>
           <a:ext cx="3838575" cy="0"/>
           <a:chOff x="1641" y="6439"/>
           <a:chExt cx="7200" cy="1800"/>
@@ -2820,7 +2805,7 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3088,74 +3073,74 @@
     <row r="1" spans="1:7" ht="60" customHeight="1"/>
     <row r="2" spans="1:7" ht="9.75" customHeight="1"/>
     <row r="3" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A3" s="100"/>
-      <c r="B3" s="101" t="s">
+      <c r="A3" s="99"/>
+      <c r="B3" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-    </row>
-    <row r="5" spans="1:7" s="92" customFormat="1" ht="12.75" customHeight="1">
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+    </row>
+    <row r="5" spans="1:7" s="91" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="5"/>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="90" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
+      <c r="C5" s="89" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="166" t="s">
+      <c r="C6" s="165" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="168">
+      <c r="C7" s="167">
         <v>42466</v>
       </c>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
     </row>
     <row r="8" spans="1:7" ht="24.75" customHeight="1">
-      <c r="C8" s="93"/>
-      <c r="D8" s="174"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="174"/>
-      <c r="G8" s="92"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="175"/>
+      <c r="E8" s="175"/>
+      <c r="F8" s="175"/>
+      <c r="G8" s="91"/>
     </row>
     <row r="9" spans="1:7" ht="18">
-      <c r="A9" s="102"/>
-      <c r="B9" s="100" t="s">
+      <c r="A9" s="101"/>
+      <c r="B9" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="102"/>
+      <c r="C9" s="101"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="169" t="s">
+      <c r="C10" s="168" t="s">
         <v>96</v>
       </c>
       <c r="E10" s="10" t="s">
@@ -3166,86 +3151,82 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="94" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="42.75" customHeight="1">
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="166" t="s">
+      <c r="C12" s="165" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="96"/>
-      <c r="C13" s="94"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="93"/>
     </row>
     <row r="14" spans="1:7" ht="18">
-      <c r="A14" s="102"/>
-      <c r="B14" s="100" t="s">
+      <c r="A14" s="101"/>
+      <c r="B14" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="102"/>
-    </row>
-    <row r="15" spans="1:7" s="103" customFormat="1" ht="16.5" customHeight="1">
+      <c r="C14" s="101"/>
+    </row>
+    <row r="15" spans="1:7" s="102" customFormat="1" ht="16.5" customHeight="1">
       <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="103" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="25.5">
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="166" t="s">
-        <v>103</v>
+      <c r="C16" s="97" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5">
-      <c r="B17" s="97" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="98" t="s">
-        <v>102</v>
+      <c r="B17" s="96" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="97" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="B18" s="97" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="98" t="s">
-        <v>101</v>
-      </c>
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="B19" s="97"/>
-      <c r="C19" s="98"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="B20" s="97"/>
-      <c r="C20" s="98"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="B21" s="97"/>
-      <c r="C21" s="98"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="97"/>
     </row>
     <row r="22" spans="1:4" ht="18">
-      <c r="A22" s="100"/>
-      <c r="B22" s="100" t="s">
+      <c r="A22" s="99"/>
+      <c r="B22" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
     </row>
     <row r="23" spans="1:4" ht="15.75">
-      <c r="A23" s="126"/>
+      <c r="A23" s="125"/>
       <c r="B23" s="9" t="s">
         <v>91</v>
       </c>
@@ -3257,83 +3238,87 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="126"/>
-      <c r="B24" s="89" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" s="173">
-        <v>42466</v>
-      </c>
-      <c r="D24" s="172"/>
+      <c r="A24" s="125"/>
+      <c r="B24" s="88" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="172">
+        <v>42465</v>
+      </c>
+      <c r="D24" s="172">
+        <v>42465</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="126"/>
-      <c r="B25" s="89" t="s">
-        <v>148</v>
-      </c>
-      <c r="C25" s="173">
+      <c r="A25" s="125"/>
+      <c r="B25" s="88" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="172">
         <v>42471</v>
       </c>
-      <c r="D25" s="172"/>
+      <c r="D25" s="172">
+        <v>42471</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="126"/>
-      <c r="B26" s="89" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="173">
+      <c r="A26" s="125"/>
+      <c r="B26" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="172">
         <v>42494</v>
       </c>
-      <c r="D26" s="172"/>
+      <c r="D26" s="171"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="126"/>
-      <c r="B27" s="89" t="s">
-        <v>150</v>
-      </c>
-      <c r="C27" s="173">
+      <c r="A27" s="125"/>
+      <c r="B27" s="88" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="172">
         <v>42501</v>
       </c>
-      <c r="D27" s="172"/>
+      <c r="D27" s="171"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" s="89"/>
-      <c r="C28" s="172"/>
-      <c r="D28" s="172"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="171"/>
+      <c r="D28" s="171"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="125"/>
-      <c r="C29" s="94"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="93"/>
     </row>
     <row r="30" spans="1:4" ht="18">
-      <c r="A30" s="102"/>
-      <c r="B30" s="100" t="s">
+      <c r="A30" s="101"/>
+      <c r="B30" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="102"/>
+      <c r="C30" s="101"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="B31" s="175" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="176"/>
+      <c r="B31" s="176" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="177"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="B32" s="99"/>
-      <c r="C32" s="99"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
     </row>
     <row r="33" spans="1:3" ht="18">
-      <c r="A33" s="102"/>
-      <c r="B33" s="100" t="s">
-        <v>106</v>
-      </c>
-      <c r="C33" s="102"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="99" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="101"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="B34" s="176" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="176"/>
+      <c r="B34" s="177" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="177"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3360,7 +3345,7 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3819,316 +3804,306 @@
     <row r="1" spans="1:7" ht="67.5" customHeight="1"/>
     <row r="2" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:7" ht="24" customHeight="1">
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="117" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="107" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B4" s="119" t="s">
+    <row r="4" spans="1:7" s="106" customFormat="1" ht="30.75" customHeight="1">
+      <c r="B4" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="180" t="s">
+      <c r="E4" s="181" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="180"/>
+      <c r="F4" s="181"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1">
-      <c r="B5" s="167" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="117" t="s">
+      <c r="B5" s="166" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="121">
+      <c r="D5" s="120">
         <v>5542583572</v>
       </c>
-      <c r="E5" s="179" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="178"/>
+      <c r="E5" s="180" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="179"/>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A6" s="116"/>
-      <c r="B6" s="167" t="s">
+      <c r="A6" s="115"/>
+      <c r="B6" s="166" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="121">
+      <c r="D6" s="120">
         <v>3318039095</v>
       </c>
-      <c r="E6" s="179" t="s">
+      <c r="E6" s="180" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="179"/>
+    </row>
+    <row r="7" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A7" s="115"/>
+      <c r="B7" s="166" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="116" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="120">
+        <v>3318039095</v>
+      </c>
+      <c r="E7" s="180" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="179"/>
+    </row>
+    <row r="8" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A8" s="115"/>
+      <c r="B8" s="166" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="116" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="120">
+        <v>3319638873</v>
+      </c>
+      <c r="E8" s="180" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="178"/>
-    </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A7" s="116"/>
-      <c r="B7" s="167" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="117" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="121">
-        <v>3318039095</v>
-      </c>
-      <c r="E7" s="179" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="178"/>
-    </row>
-    <row r="8" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A8" s="116"/>
-      <c r="B8" s="167" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="117" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="121">
-        <v>3319638873</v>
-      </c>
-      <c r="E8" s="179" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="178"/>
+      <c r="F8" s="179"/>
     </row>
     <row r="9" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A9" s="116"/>
-      <c r="B9" s="167" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="117" t="s">
+      <c r="A9" s="115"/>
+      <c r="B9" s="166" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="121">
+      <c r="D9" s="120">
         <v>3312430761</v>
       </c>
-      <c r="E9" s="179" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="178"/>
+      <c r="E9" s="180" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="179"/>
     </row>
     <row r="10" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A10" s="116"/>
-      <c r="B10" s="167" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="117" t="s">
+      <c r="A10" s="115"/>
+      <c r="B10" s="166" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="121">
+      <c r="D10" s="120">
         <v>3310739239</v>
       </c>
-      <c r="E10" s="179" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="178"/>
+      <c r="E10" s="180" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="179"/>
     </row>
     <row r="11" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A11" s="116"/>
-      <c r="B11" s="167" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="117" t="s">
+      <c r="A11" s="115"/>
+      <c r="B11" s="166" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="121">
+      <c r="D11" s="120">
         <v>3310739239</v>
       </c>
-      <c r="E11" s="179" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="178"/>
+      <c r="E11" s="180" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="179"/>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="112"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="111"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:7" ht="23.25" customHeight="1">
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="117" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="107" customFormat="1" ht="23.25" customHeight="1">
-      <c r="B14" s="120" t="s">
+    <row r="14" spans="1:7" s="106" customFormat="1" ht="23.25" customHeight="1">
+      <c r="B14" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="119" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="120" t="s">
+      <c r="D14" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="120" t="s">
+      <c r="E14" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="115"/>
-    </row>
-    <row r="15" spans="1:7" ht="25.5">
-      <c r="B15" s="122" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="170" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="124"/>
-      <c r="G15" s="113"/>
-    </row>
-    <row r="16" spans="1:7" ht="25.5">
-      <c r="B16" s="122" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="170" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="123"/>
-      <c r="E16" s="124"/>
-    </row>
-    <row r="17" spans="2:7" ht="25.5">
-      <c r="B17" s="122" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="170" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="123"/>
-      <c r="E17" s="124"/>
+      <c r="G14" s="114"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="121" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="169"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="123"/>
+      <c r="G15" s="112"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="121"/>
+      <c r="C16" s="169"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="123"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="121"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="123"/>
     </row>
     <row r="18" spans="2:7" ht="20.25" customHeight="1">
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
     </row>
     <row r="19" spans="2:7" ht="25.5">
-      <c r="B19" s="111" t="s">
+      <c r="B19" s="110" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:7" s="107" customFormat="1" ht="33.75" customHeight="1">
-      <c r="B20" s="119" t="s">
+    <row r="20" spans="2:7" s="106" customFormat="1" ht="33.75" customHeight="1">
+      <c r="B20" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="119" t="s">
+      <c r="C20" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="119" t="s">
+      <c r="D20" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="180" t="s">
+      <c r="E20" s="181" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="180"/>
+      <c r="F20" s="181"/>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="167" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="121"/>
-      <c r="E21" s="179" t="s">
-        <v>153</v>
-      </c>
-      <c r="F21" s="178"/>
+      <c r="B21" s="166" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="120" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="120"/>
+      <c r="E21" s="180" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="179"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="167"/>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
-      <c r="E22" s="177"/>
-      <c r="F22" s="178"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="178"/>
+      <c r="F22" s="179"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="167"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="177"/>
-      <c r="F23" s="178"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="178"/>
+      <c r="F23" s="179"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="167"/>
-      <c r="C24" s="121"/>
-      <c r="D24" s="121"/>
-      <c r="E24" s="177"/>
-      <c r="F24" s="178"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="178"/>
+      <c r="F24" s="179"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="167"/>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="177"/>
-      <c r="F25" s="178"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="178"/>
+      <c r="F25" s="179"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="167"/>
-      <c r="C26" s="121"/>
-      <c r="D26" s="121"/>
-      <c r="E26" s="177"/>
-      <c r="F26" s="178"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="120"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="179"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="167"/>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="177"/>
-      <c r="F27" s="178"/>
+      <c r="B27" s="166"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="178"/>
+      <c r="F27" s="179"/>
     </row>
     <row r="28" spans="2:7" ht="15.75">
-      <c r="C28" s="107"/>
-      <c r="D28" s="108"/>
-      <c r="E28" s="109"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="107"/>
+      <c r="E28" s="108"/>
     </row>
     <row r="29" spans="2:7" ht="15.75">
-      <c r="C29" s="107"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="109"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="108"/>
     </row>
     <row r="30" spans="2:7" ht="15.75">
-      <c r="C30" s="107"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="109"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="107"/>
+      <c r="E30" s="108"/>
     </row>
     <row r="31" spans="2:7" ht="15.75">
-      <c r="C31" s="107"/>
-      <c r="D31" s="108"/>
-      <c r="E31" s="109"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="108"/>
     </row>
     <row r="32" spans="2:7" ht="15.75">
-      <c r="C32" s="107"/>
-      <c r="D32" s="108"/>
-      <c r="E32" s="109"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="108"/>
     </row>
     <row r="33" spans="3:5" ht="15.75">
-      <c r="C33" s="107"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="110"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="109"/>
     </row>
     <row r="34" spans="3:5" ht="15.75">
-      <c r="C34" s="107"/>
-      <c r="D34" s="108"/>
-      <c r="E34" s="109"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="108"/>
     </row>
     <row r="35" spans="3:5" ht="15.75">
-      <c r="C35" s="107"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="109"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="107"/>
+      <c r="E35" s="108"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -4999,58 +4974,64 @@
     </row>
     <row r="5" spans="1:12" ht="49.5">
       <c r="B5" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="171" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="170" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="171" t="s">
-        <v>118</v>
+      <c r="D5" s="170" t="s">
+        <v>109</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:12" ht="33">
       <c r="B6" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="171" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="170" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="171"/>
+      <c r="D6" s="170" t="s">
+        <v>142</v>
+      </c>
       <c r="E6" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" s="16"/>
+        <v>114</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>150</v>
+      </c>
       <c r="G6" s="18"/>
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" ht="33">
       <c r="B7" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="171" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="171"/>
+      <c r="C7" s="170" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="170" t="s">
+        <v>95</v>
+      </c>
       <c r="E7" s="16" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G7" s="18"/>
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" ht="16.5">
       <c r="B8" s="15"/>
-      <c r="C8" s="171"/>
-      <c r="D8" s="171"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="170"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="18"/>
@@ -5273,7 +5254,7 @@
     </row>
     <row r="5" spans="2:11" ht="16.5">
       <c r="B5" s="27" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>43</v>
@@ -5282,8 +5263,12 @@
       <c r="E5" s="28">
         <v>5</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="F5" s="173">
+        <v>42457</v>
+      </c>
+      <c r="G5" s="173">
+        <v>42457</v>
+      </c>
       <c r="H5" s="29"/>
       <c r="K5" s="3" t="s">
         <v>43</v>
@@ -5291,7 +5276,7 @@
     </row>
     <row r="6" spans="2:11" ht="16.5">
       <c r="B6" s="27" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>42</v>
@@ -5300,8 +5285,12 @@
       <c r="E6" s="28">
         <v>5</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="173">
+        <v>42457</v>
+      </c>
+      <c r="G6" s="173">
+        <v>42457</v>
+      </c>
       <c r="H6" s="29"/>
       <c r="K6" s="3" t="s">
         <v>42</v>
@@ -5309,7 +5298,7 @@
     </row>
     <row r="7" spans="2:11" ht="33">
       <c r="B7" s="27" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>42</v>
@@ -5318,8 +5307,12 @@
       <c r="E7" s="28">
         <v>5</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="F7" s="173">
+        <v>42457</v>
+      </c>
+      <c r="G7" s="173">
+        <v>42457</v>
+      </c>
       <c r="H7" s="29"/>
       <c r="K7" s="3" t="s">
         <v>44</v>
@@ -5327,7 +5320,7 @@
     </row>
     <row r="8" spans="2:11" ht="16.5">
       <c r="B8" s="27" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>42</v>
@@ -5336,14 +5329,18 @@
       <c r="E8" s="28">
         <v>2</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="F8" s="173">
+        <v>42457</v>
+      </c>
+      <c r="G8" s="173">
+        <v>42457</v>
+      </c>
       <c r="H8" s="29"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="33">
       <c r="B9" s="27" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>44</v>
@@ -5352,8 +5349,12 @@
       <c r="E9" s="28">
         <v>1</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="F9" s="173">
+        <v>42457</v>
+      </c>
+      <c r="G9" s="173">
+        <v>42457</v>
+      </c>
       <c r="H9" s="29"/>
     </row>
     <row r="10" spans="2:11" ht="16.5">
@@ -5437,7 +5438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IZ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5466,8 +5467,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:260" ht="68.25" customHeight="1">
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
     </row>
     <row r="2" spans="1:260" ht="18" customHeight="1">
       <c r="A2" s="34"/>
@@ -5547,32 +5548,32 @@
       <c r="J4" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="181" t="s">
+      <c r="L4" s="182" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="130">
+      <c r="M4" s="129">
         <v>5</v>
       </c>
-      <c r="N4" s="147">
+      <c r="N4" s="146">
         <v>5</v>
       </c>
-      <c r="O4" s="131">
+      <c r="O4" s="130">
         <v>10</v>
       </c>
-      <c r="P4" s="132">
+      <c r="P4" s="131">
         <v>15</v>
       </c>
-      <c r="Q4" s="133">
+      <c r="Q4" s="132">
         <v>20</v>
       </c>
-      <c r="R4" s="134">
+      <c r="R4" s="133">
         <v>25</v>
       </c>
-      <c r="S4" s="127"/>
-      <c r="T4" s="183" t="s">
+      <c r="S4" s="126"/>
+      <c r="T4" s="184" t="s">
         <v>62</v>
       </c>
-      <c r="U4" s="184"/>
+      <c r="U4" s="185"/>
       <c r="AD4" s="31" t="s">
         <v>46</v>
       </c>
@@ -5585,7 +5586,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C5" s="82">
         <v>3</v>
@@ -5598,42 +5599,44 @@
         <v>9</v>
       </c>
       <c r="F5" s="81" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G5" s="81" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H5" s="82" t="s">
         <v>95</v>
       </c>
       <c r="I5" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="J5" s="83"/>
-      <c r="L5" s="181"/>
-      <c r="M5" s="130">
+        <v>132</v>
+      </c>
+      <c r="J5" s="174" t="s">
+        <v>150</v>
+      </c>
+      <c r="L5" s="182"/>
+      <c r="M5" s="129">
         <v>4</v>
       </c>
-      <c r="N5" s="148">
+      <c r="N5" s="147">
         <v>4</v>
       </c>
-      <c r="O5" s="135">
+      <c r="O5" s="134">
         <v>8</v>
       </c>
-      <c r="P5" s="136">
+      <c r="P5" s="135">
         <v>12</v>
       </c>
-      <c r="Q5" s="134">
+      <c r="Q5" s="133">
         <v>16</v>
       </c>
-      <c r="R5" s="134">
+      <c r="R5" s="133">
         <v>20</v>
       </c>
-      <c r="S5" s="127"/>
-      <c r="T5" s="153" t="s">
+      <c r="S5" s="126"/>
+      <c r="T5" s="152" t="s">
         <v>63</v>
       </c>
-      <c r="U5" s="154" t="s">
+      <c r="U5" s="153" t="s">
         <v>56</v>
       </c>
       <c r="IR5" s="32" t="s">
@@ -5667,12 +5670,12 @@
       </c>
     </row>
     <row r="6" spans="1:260" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A6" s="84">
+      <c r="A6" s="83">
         <f>A5+1</f>
         <v>2</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C6" s="82">
         <v>4</v>
@@ -5685,42 +5688,44 @@
         <v>12</v>
       </c>
       <c r="F6" s="81" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H6" s="82" t="s">
         <v>95</v>
       </c>
       <c r="I6" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="J6" s="83"/>
-      <c r="L6" s="181"/>
-      <c r="M6" s="130">
+        <v>132</v>
+      </c>
+      <c r="J6" s="174" t="s">
+        <v>150</v>
+      </c>
+      <c r="L6" s="182"/>
+      <c r="M6" s="129">
         <v>3</v>
       </c>
-      <c r="N6" s="149">
+      <c r="N6" s="148">
         <v>3</v>
       </c>
-      <c r="O6" s="137">
+      <c r="O6" s="136">
         <v>6</v>
       </c>
-      <c r="P6" s="131">
+      <c r="P6" s="130">
         <v>9</v>
       </c>
-      <c r="Q6" s="134">
+      <c r="Q6" s="133">
         <v>12</v>
       </c>
-      <c r="R6" s="134">
+      <c r="R6" s="133">
         <v>15</v>
       </c>
-      <c r="S6" s="127"/>
-      <c r="T6" s="155">
+      <c r="S6" s="126"/>
+      <c r="T6" s="154">
         <v>1</v>
       </c>
-      <c r="U6" s="156" t="s">
+      <c r="U6" s="155" t="s">
         <v>68</v>
       </c>
       <c r="IR6" s="32"/>
@@ -5752,12 +5757,12 @@
       </c>
     </row>
     <row r="7" spans="1:260" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A7" s="84">
+      <c r="A7" s="83">
         <f t="shared" ref="A7:A20" si="1">A6+1</f>
         <v>3</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C7" s="82">
         <v>2</v>
@@ -5765,45 +5770,49 @@
       <c r="D7" s="82">
         <v>4</v>
       </c>
-      <c r="E7" s="85">
+      <c r="E7" s="84">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F7" s="81" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G7" s="81" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" s="82"/>
+        <v>129</v>
+      </c>
+      <c r="H7" s="82" t="s">
+        <v>95</v>
+      </c>
       <c r="I7" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="J7" s="86"/>
-      <c r="L7" s="181"/>
-      <c r="M7" s="130">
+        <v>132</v>
+      </c>
+      <c r="J7" s="174" t="s">
+        <v>150</v>
+      </c>
+      <c r="L7" s="182"/>
+      <c r="M7" s="129">
         <v>2</v>
       </c>
-      <c r="N7" s="150">
+      <c r="N7" s="149">
         <v>2</v>
       </c>
-      <c r="O7" s="139">
+      <c r="O7" s="138">
         <v>4</v>
       </c>
-      <c r="P7" s="140">
+      <c r="P7" s="139">
         <v>6</v>
       </c>
-      <c r="Q7" s="141">
+      <c r="Q7" s="140">
         <v>8</v>
       </c>
-      <c r="R7" s="131">
+      <c r="R7" s="130">
         <v>10</v>
       </c>
-      <c r="S7" s="152"/>
-      <c r="T7" s="155">
+      <c r="S7" s="151"/>
+      <c r="T7" s="154">
         <v>2</v>
       </c>
-      <c r="U7" s="157" t="s">
+      <c r="U7" s="156" t="s">
         <v>69</v>
       </c>
       <c r="IR7" s="32"/>
@@ -5835,12 +5844,12 @@
       </c>
     </row>
     <row r="8" spans="1:260" ht="71.25" customHeight="1" thickBot="1">
-      <c r="A8" s="84">
+      <c r="A8" s="83">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B8" s="81" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C8" s="82">
         <v>5</v>
@@ -5848,47 +5857,49 @@
       <c r="D8" s="82">
         <v>2</v>
       </c>
-      <c r="E8" s="85">
+      <c r="E8" s="84">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F8" s="81" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H8" s="82" t="s">
         <v>95</v>
       </c>
       <c r="I8" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" s="86"/>
-      <c r="L8" s="181"/>
-      <c r="M8" s="130">
+        <v>132</v>
+      </c>
+      <c r="J8" s="174" t="s">
+        <v>150</v>
+      </c>
+      <c r="L8" s="182"/>
+      <c r="M8" s="129">
         <v>1</v>
       </c>
-      <c r="N8" s="151">
+      <c r="N8" s="150">
         <v>1</v>
       </c>
-      <c r="O8" s="142">
+      <c r="O8" s="141">
         <v>2</v>
       </c>
-      <c r="P8" s="138">
+      <c r="P8" s="137">
         <v>3</v>
       </c>
-      <c r="Q8" s="143">
+      <c r="Q8" s="142">
         <v>4</v>
       </c>
-      <c r="R8" s="137">
+      <c r="R8" s="136">
         <v>5</v>
       </c>
-      <c r="S8" s="127"/>
-      <c r="T8" s="155">
+      <c r="S8" s="126"/>
+      <c r="T8" s="154">
         <v>3</v>
       </c>
-      <c r="U8" s="157" t="s">
+      <c r="U8" s="156" t="s">
         <v>70</v>
       </c>
       <c r="IR8" s="32"/>
@@ -5920,12 +5931,12 @@
       </c>
     </row>
     <row r="9" spans="1:260" ht="53.25" customHeight="1">
-      <c r="A9" s="84">
+      <c r="A9" s="83">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B9" s="81" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C9" s="82">
         <v>3</v>
@@ -5933,45 +5944,47 @@
       <c r="D9" s="82">
         <v>1</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="84">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F9" s="81" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H9" s="82" t="s">
         <v>95</v>
       </c>
       <c r="I9" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="J9" s="86"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="144"/>
-      <c r="N9" s="145">
+        <v>132</v>
+      </c>
+      <c r="J9" s="174" t="s">
+        <v>150</v>
+      </c>
+      <c r="L9" s="129"/>
+      <c r="M9" s="143"/>
+      <c r="N9" s="144">
         <v>1</v>
       </c>
-      <c r="O9" s="146">
+      <c r="O9" s="145">
         <v>2</v>
       </c>
-      <c r="P9" s="145">
+      <c r="P9" s="144">
         <v>3</v>
       </c>
-      <c r="Q9" s="146">
+      <c r="Q9" s="145">
         <v>4</v>
       </c>
-      <c r="R9" s="145">
+      <c r="R9" s="144">
         <v>5</v>
       </c>
       <c r="S9" s="37"/>
-      <c r="T9" s="155">
+      <c r="T9" s="154">
         <v>4</v>
       </c>
-      <c r="U9" s="157" t="s">
+      <c r="U9" s="156" t="s">
         <v>77</v>
       </c>
       <c r="IR9" s="32"/>
@@ -6003,36 +6016,36 @@
       </c>
     </row>
     <row r="10" spans="1:260" ht="18" customHeight="1">
-      <c r="A10" s="84">
+      <c r="A10" s="83">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B10" s="81"/>
       <c r="C10" s="82"/>
       <c r="D10" s="82"/>
-      <c r="E10" s="85">
+      <c r="E10" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="87"/>
+      <c r="F10" s="86"/>
       <c r="G10" s="81"/>
       <c r="H10" s="82"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="86"/>
-      <c r="L10" s="130"/>
-      <c r="M10" s="144"/>
-      <c r="N10" s="182" t="s">
+      <c r="I10" s="84"/>
+      <c r="J10" s="85"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="143"/>
+      <c r="N10" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="182"/>
-      <c r="P10" s="182"/>
-      <c r="Q10" s="182"/>
-      <c r="R10" s="182"/>
+      <c r="O10" s="183"/>
+      <c r="P10" s="183"/>
+      <c r="Q10" s="183"/>
+      <c r="R10" s="183"/>
       <c r="S10" s="38"/>
-      <c r="T10" s="155">
+      <c r="T10" s="154">
         <v>5</v>
       </c>
-      <c r="U10" s="157" t="s">
+      <c r="U10" s="156" t="s">
         <v>71</v>
       </c>
       <c r="IR10" s="56"/>
@@ -6055,34 +6068,34 @@
       </c>
     </row>
     <row r="11" spans="1:260" ht="18" customHeight="1">
-      <c r="A11" s="84">
+      <c r="A11" s="83">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B11" s="81"/>
       <c r="C11" s="82"/>
       <c r="D11" s="82"/>
-      <c r="E11" s="85">
+      <c r="E11" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="87"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="81"/>
       <c r="H11" s="82"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="86"/>
-      <c r="L11" s="129"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="85"/>
+      <c r="L11" s="128"/>
       <c r="M11" s="38"/>
-      <c r="N11" s="129"/>
+      <c r="N11" s="128"/>
       <c r="O11" s="38"/>
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
       <c r="S11" s="38"/>
-      <c r="T11" s="153" t="s">
+      <c r="T11" s="152" t="s">
         <v>63</v>
       </c>
-      <c r="U11" s="158" t="s">
+      <c r="U11" s="157" t="s">
         <v>50</v>
       </c>
       <c r="IR11" s="56"/>
@@ -6105,23 +6118,23 @@
       </c>
     </row>
     <row r="12" spans="1:260" ht="18" customHeight="1">
-      <c r="A12" s="84">
+      <c r="A12" s="83">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B12" s="81"/>
       <c r="C12" s="82"/>
       <c r="D12" s="82"/>
-      <c r="E12" s="85">
+      <c r="E12" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="87"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="81"/>
       <c r="H12" s="82"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="86"/>
-      <c r="L12" s="129"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="85"/>
+      <c r="L12" s="128"/>
       <c r="M12" s="38"/>
       <c r="N12" s="38"/>
       <c r="O12" s="38"/>
@@ -6129,10 +6142,10 @@
       <c r="Q12" s="38"/>
       <c r="R12" s="38"/>
       <c r="S12" s="38"/>
-      <c r="T12" s="155">
+      <c r="T12" s="154">
         <v>1</v>
       </c>
-      <c r="U12" s="159" t="s">
+      <c r="U12" s="158" t="s">
         <v>73</v>
       </c>
       <c r="IR12" s="56"/>
@@ -6147,23 +6160,23 @@
       <c r="IY12" s="59"/>
     </row>
     <row r="13" spans="1:260" ht="18" customHeight="1">
-      <c r="A13" s="84">
+      <c r="A13" s="83">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B13" s="81"/>
       <c r="C13" s="82"/>
       <c r="D13" s="82"/>
-      <c r="E13" s="85">
+      <c r="E13" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="87"/>
+      <c r="F13" s="86"/>
       <c r="G13" s="81"/>
       <c r="H13" s="82"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="86"/>
-      <c r="L13" s="129"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
+      <c r="L13" s="128"/>
       <c r="M13" s="38"/>
       <c r="N13" s="38"/>
       <c r="O13" s="38"/>
@@ -6171,10 +6184,10 @@
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
-      <c r="T13" s="155">
+      <c r="T13" s="154">
         <v>2</v>
       </c>
-      <c r="U13" s="156" t="s">
+      <c r="U13" s="155" t="s">
         <v>72</v>
       </c>
       <c r="IR13" s="56"/>
@@ -6187,23 +6200,23 @@
       <c r="IY13" s="49"/>
     </row>
     <row r="14" spans="1:260" ht="18" customHeight="1">
-      <c r="A14" s="84">
+      <c r="A14" s="83">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B14" s="81"/>
       <c r="C14" s="82"/>
       <c r="D14" s="82"/>
-      <c r="E14" s="85">
+      <c r="E14" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="87"/>
+      <c r="F14" s="86"/>
       <c r="G14" s="81"/>
       <c r="H14" s="82"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="86"/>
-      <c r="L14" s="129"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="85"/>
+      <c r="L14" s="128"/>
       <c r="M14" s="38"/>
       <c r="N14" s="38"/>
       <c r="O14" s="38"/>
@@ -6211,10 +6224,10 @@
       <c r="Q14" s="38"/>
       <c r="R14" s="38"/>
       <c r="S14" s="38"/>
-      <c r="T14" s="155">
+      <c r="T14" s="154">
         <v>3</v>
       </c>
-      <c r="U14" s="157" t="s">
+      <c r="U14" s="156" t="s">
         <v>74</v>
       </c>
       <c r="IR14" s="56"/>
@@ -6227,22 +6240,22 @@
       <c r="IY14" s="61"/>
     </row>
     <row r="15" spans="1:260" ht="18" customHeight="1">
-      <c r="A15" s="84">
+      <c r="A15" s="83">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B15" s="81"/>
       <c r="C15" s="82"/>
       <c r="D15" s="82"/>
-      <c r="E15" s="85">
+      <c r="E15" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="87"/>
+      <c r="F15" s="86"/>
       <c r="G15" s="81"/>
       <c r="H15" s="82"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="86"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="85"/>
       <c r="L15" s="51"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
@@ -6251,10 +6264,10 @@
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
       <c r="S15" s="38"/>
-      <c r="T15" s="155">
+      <c r="T15" s="154">
         <v>4</v>
       </c>
-      <c r="U15" s="157" t="s">
+      <c r="U15" s="156" t="s">
         <v>75</v>
       </c>
       <c r="IR15" s="62" t="s">
@@ -6269,22 +6282,22 @@
       <c r="IY15" s="61"/>
     </row>
     <row r="16" spans="1:260" ht="18" customHeight="1">
-      <c r="A16" s="84">
+      <c r="A16" s="83">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B16" s="81"/>
       <c r="C16" s="82"/>
       <c r="D16" s="82"/>
-      <c r="E16" s="85">
+      <c r="E16" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="87"/>
+      <c r="F16" s="86"/>
       <c r="G16" s="81"/>
       <c r="H16" s="82"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="86"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="85"/>
       <c r="L16" s="51"/>
       <c r="M16" s="38"/>
       <c r="N16" s="38"/>
@@ -6293,10 +6306,10 @@
       <c r="Q16" s="38"/>
       <c r="R16" s="38"/>
       <c r="S16" s="38"/>
-      <c r="T16" s="155">
+      <c r="T16" s="154">
         <v>5</v>
       </c>
-      <c r="U16" s="159" t="s">
+      <c r="U16" s="158" t="s">
         <v>76</v>
       </c>
       <c r="IR16" s="56" t="s">
@@ -6313,22 +6326,22 @@
       <c r="IY16" s="64"/>
     </row>
     <row r="17" spans="1:259" ht="18" customHeight="1">
-      <c r="A17" s="84">
+      <c r="A17" s="83">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B17" s="81"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
-      <c r="E17" s="85">
+      <c r="E17" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="87"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="81"/>
       <c r="H17" s="82"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="86"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="85"/>
       <c r="L17" s="51"/>
       <c r="M17" s="38"/>
       <c r="N17" s="38"/>
@@ -6337,8 +6350,8 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
       <c r="S17" s="38"/>
-      <c r="T17" s="160"/>
-      <c r="U17" s="158" t="s">
+      <c r="T17" s="159"/>
+      <c r="U17" s="157" t="s">
         <v>67</v>
       </c>
       <c r="IR17" s="56" t="s">
@@ -6355,22 +6368,22 @@
       <c r="IY17" s="64"/>
     </row>
     <row r="18" spans="1:259" ht="18" customHeight="1">
-      <c r="A18" s="84">
+      <c r="A18" s="83">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B18" s="81"/>
       <c r="C18" s="82"/>
       <c r="D18" s="82"/>
-      <c r="E18" s="85">
+      <c r="E18" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="87"/>
+      <c r="F18" s="86"/>
       <c r="G18" s="81"/>
       <c r="H18" s="82"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="86"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="85"/>
       <c r="L18" s="51"/>
       <c r="M18" s="38"/>
       <c r="N18" s="38"/>
@@ -6379,8 +6392,8 @@
       <c r="Q18" s="38"/>
       <c r="R18" s="38"/>
       <c r="S18" s="38"/>
-      <c r="T18" s="161"/>
-      <c r="U18" s="162" t="s">
+      <c r="T18" s="160"/>
+      <c r="U18" s="161" t="s">
         <v>64</v>
       </c>
       <c r="IR18" s="56" t="s">
@@ -6397,22 +6410,22 @@
       <c r="IY18" s="64"/>
     </row>
     <row r="19" spans="1:259" ht="18" customHeight="1" thickBot="1">
-      <c r="A19" s="84">
+      <c r="A19" s="83">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B19" s="81"/>
       <c r="C19" s="82"/>
       <c r="D19" s="82"/>
-      <c r="E19" s="85">
+      <c r="E19" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="87"/>
+      <c r="F19" s="86"/>
       <c r="G19" s="81"/>
       <c r="H19" s="82"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="86"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="85"/>
       <c r="L19" s="51"/>
       <c r="M19" s="38"/>
       <c r="N19" s="38"/>
@@ -6421,8 +6434,8 @@
       <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
       <c r="S19" s="38"/>
-      <c r="T19" s="163"/>
-      <c r="U19" s="162" t="s">
+      <c r="T19" s="162"/>
+      <c r="U19" s="161" t="s">
         <v>65</v>
       </c>
       <c r="IR19" s="65"/>
@@ -6435,22 +6448,22 @@
       <c r="IY19" s="68"/>
     </row>
     <row r="20" spans="1:259" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="84">
+      <c r="A20" s="83">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B20" s="81"/>
       <c r="C20" s="82"/>
       <c r="D20" s="82"/>
-      <c r="E20" s="85">
+      <c r="E20" s="84">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="87"/>
+      <c r="F20" s="86"/>
       <c r="G20" s="81"/>
       <c r="H20" s="82"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="86"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="85"/>
       <c r="L20" s="51"/>
       <c r="M20" s="38"/>
       <c r="N20" s="38"/>
@@ -6459,8 +6472,8 @@
       <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
       <c r="S20" s="38"/>
-      <c r="T20" s="164"/>
-      <c r="U20" s="165" t="s">
+      <c r="T20" s="163"/>
+      <c r="U20" s="164" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>